<commit_message>
Van der Steur toegevoegd
</commit_message>
<xml_diff>
--- a/Data/Extra info verwijderde namen.xlsx
+++ b/Data/Extra info verwijderde namen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alielassche/Dropbox/Student-assistentschap/Netwerken_huwelijksgedichten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alielassche/Documents/GitHub/netwerk-huwelijksgedichten/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3488B5-9D3B-2B47-A269-5A676E953103}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9290D42B-B445-9942-991F-C50E3D6698AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="2" xr2:uid="{91DC8FCD-999E-C04C-A5B7-D30830052C4B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{91DC8FCD-999E-C04C-A5B7-D30830052C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Drukkers" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="592">
   <si>
     <t>Goeree</t>
   </si>
@@ -1783,13 +1783,34 @@
   </si>
   <si>
     <t>Boudewijn Janssoon van der (II) Aa</t>
+  </si>
+  <si>
+    <t>Erven J. Lescailje en Dirk Rank</t>
+  </si>
+  <si>
+    <t>Gerrit Muntendam</t>
+  </si>
+  <si>
+    <t>Gerrit (wed) Muntendam</t>
+  </si>
+  <si>
+    <t>Gerrit (wed.) Muntendam</t>
+  </si>
+  <si>
+    <t>G. Muntendam (wed)</t>
+  </si>
+  <si>
+    <t>Hendrik Bruyn</t>
+  </si>
+  <si>
+    <t>Willem en David Goeree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1838,6 +1859,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1906,7 +1933,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1942,6 +1969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2257,10 +2285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC8214C-B4FA-7B44-AB5D-D8A034BCE402}">
-  <dimension ref="A1:D393"/>
+  <dimension ref="A1:D409"/>
   <sheetViews>
-    <sheetView topLeftCell="A279" workbookViewId="0">
-      <selection activeCell="C324" sqref="C324"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2477,18 +2505,18 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>5</v>
+        <v>3975</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -2496,13 +2524,10 @@
       <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -2516,7 +2541,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>147</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -2524,10 +2549,13 @@
       <c r="C22" t="s">
         <v>6</v>
       </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>403</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2538,7 +2566,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>437</v>
+        <v>403</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -2546,13 +2574,10 @@
       <c r="C24" t="s">
         <v>6</v>
       </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -2566,7 +2591,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2580,7 +2605,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -2594,7 +2619,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -2608,7 +2633,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>497</v>
+        <v>441</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -2616,10 +2641,13 @@
       <c r="C29" t="s">
         <v>6</v>
       </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>1245</v>
+        <v>497</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -2630,7 +2658,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -2641,7 +2669,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -2652,7 +2680,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -2663,7 +2691,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
@@ -2674,7 +2702,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
@@ -2685,7 +2713,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
@@ -2696,7 +2724,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
@@ -2707,7 +2735,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -2718,7 +2746,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
@@ -2729,7 +2757,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -2740,7 +2768,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
@@ -2751,7 +2779,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
@@ -2762,7 +2790,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
@@ -2773,7 +2801,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
@@ -2784,7 +2812,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
@@ -2795,7 +2823,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -2806,7 +2834,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
@@ -2817,7 +2845,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
@@ -2828,7 +2856,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
@@ -2839,7 +2867,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
@@ -2850,7 +2878,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
@@ -2861,7 +2889,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
@@ -2872,7 +2900,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
@@ -2883,7 +2911,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
@@ -2894,7 +2922,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -2905,7 +2933,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
@@ -2916,7 +2944,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
@@ -2927,7 +2955,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="B58" t="s">
         <v>5</v>
@@ -2938,7 +2966,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
@@ -2949,7 +2977,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
@@ -2960,7 +2988,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
@@ -2971,7 +2999,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
@@ -2982,7 +3010,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="B63" t="s">
         <v>5</v>
@@ -2993,7 +3021,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="B64" t="s">
         <v>5</v>
@@ -3004,7 +3032,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
@@ -3015,7 +3043,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
@@ -3026,7 +3054,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
@@ -3037,7 +3065,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="B68" t="s">
         <v>5</v>
@@ -3048,7 +3076,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B69" t="s">
         <v>5</v>
@@ -3059,7 +3087,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B70" t="s">
         <v>5</v>
@@ -3070,7 +3098,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
@@ -3081,7 +3109,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
@@ -3092,7 +3120,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
@@ -3103,7 +3131,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="B74" t="s">
         <v>5</v>
@@ -3114,7 +3142,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
@@ -3125,7 +3153,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
@@ -3136,7 +3164,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
@@ -3147,7 +3175,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
@@ -3158,7 +3186,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
@@ -3169,7 +3197,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="B80" t="s">
         <v>5</v>
@@ -3180,7 +3208,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
@@ -3191,7 +3219,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
@@ -3202,7 +3230,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="B83" t="s">
         <v>5</v>
@@ -3213,7 +3241,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="B84" t="s">
         <v>5</v>
@@ -3224,7 +3252,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
@@ -3235,7 +3263,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
@@ -3246,7 +3274,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
@@ -3257,7 +3285,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B88" t="s">
         <v>5</v>
@@ -3268,7 +3296,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="B89" t="s">
         <v>5</v>
@@ -3279,7 +3307,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B90" t="s">
         <v>5</v>
@@ -3290,7 +3318,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B91" t="s">
         <v>5</v>
@@ -3301,7 +3329,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
@@ -3312,7 +3340,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B93" t="s">
         <v>5</v>
@@ -3323,7 +3351,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="B94" t="s">
         <v>5</v>
@@ -3334,7 +3362,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
@@ -3345,7 +3373,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="B96" t="s">
         <v>5</v>
@@ -3356,18 +3384,18 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>379</v>
+        <v>1311</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>1243</v>
+        <v>379</v>
       </c>
       <c r="B98" t="s">
         <v>5</v>
@@ -3378,7 +3406,7 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B99" t="s">
         <v>5</v>
@@ -3389,43 +3417,40 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>1241</v>
+        <v>1244</v>
       </c>
       <c r="B100" t="s">
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>19</v>
+        <v>1242</v>
       </c>
       <c r="B102" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>13</v>
-      </c>
-      <c r="D102" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>515</v>
+        <v>19</v>
       </c>
       <c r="B103" t="s">
         <v>11</v>
@@ -3439,7 +3464,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B104" t="s">
         <v>11</v>
@@ -3453,7 +3478,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B105" t="s">
         <v>11</v>
@@ -3462,23 +3487,26 @@
         <v>13</v>
       </c>
       <c r="D105" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>17</v>
+        <v>517</v>
       </c>
       <c r="B106" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C106" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D106" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>724</v>
+        <v>17</v>
       </c>
       <c r="B107" t="s">
         <v>12</v>
@@ -3489,18 +3517,18 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>52</v>
+        <v>724</v>
       </c>
       <c r="B108" t="s">
         <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B109" t="s">
         <v>12</v>
@@ -3511,7 +3539,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B110" t="s">
         <v>12</v>
@@ -3522,7 +3550,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B111" t="s">
         <v>12</v>
@@ -3533,7 +3561,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B112" t="s">
         <v>12</v>
@@ -3544,7 +3572,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B113" t="s">
         <v>12</v>
@@ -3555,7 +3583,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B114" t="s">
         <v>12</v>
@@ -3566,7 +3594,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B115" t="s">
         <v>12</v>
@@ -3577,7 +3605,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B116" t="s">
         <v>12</v>
@@ -3587,8 +3615,8 @@
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="3">
-        <v>67</v>
+      <c r="A117">
+        <v>63</v>
       </c>
       <c r="B117" t="s">
         <v>12</v>
@@ -3599,7 +3627,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B118" t="s">
         <v>12</v>
@@ -3610,7 +3638,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B119" t="s">
         <v>12</v>
@@ -3620,8 +3648,8 @@
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120">
-        <v>82</v>
+      <c r="A120" s="3">
+        <v>75</v>
       </c>
       <c r="B120" t="s">
         <v>12</v>
@@ -3632,7 +3660,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B121" t="s">
         <v>12</v>
@@ -3643,7 +3671,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B122" t="s">
         <v>12</v>
@@ -3653,8 +3681,8 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="3">
-        <v>92</v>
+      <c r="A123">
+        <v>91</v>
       </c>
       <c r="B123" t="s">
         <v>12</v>
@@ -3664,8 +3692,8 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124">
-        <v>95</v>
+      <c r="A124" s="3">
+        <v>92</v>
       </c>
       <c r="B124" t="s">
         <v>12</v>
@@ -3676,7 +3704,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B125" t="s">
         <v>12</v>
@@ -3687,7 +3715,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B126" t="s">
         <v>12</v>
@@ -3698,7 +3726,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="B127" t="s">
         <v>12</v>
@@ -3709,7 +3737,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B128" t="s">
         <v>12</v>
@@ -3720,7 +3748,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B129" t="s">
         <v>12</v>
@@ -3731,7 +3759,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="B130" t="s">
         <v>12</v>
@@ -3742,7 +3770,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B131" t="s">
         <v>12</v>
@@ -3753,7 +3781,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B132" t="s">
         <v>12</v>
@@ -3764,7 +3792,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B133" t="s">
         <v>12</v>
@@ -3775,7 +3803,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B134" t="s">
         <v>12</v>
@@ -3785,8 +3813,8 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="3">
-        <v>174</v>
+      <c r="A135">
+        <v>173</v>
       </c>
       <c r="B135" t="s">
         <v>12</v>
@@ -3797,7 +3825,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B136" t="s">
         <v>12</v>
@@ -3807,8 +3835,8 @@
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137">
-        <v>176</v>
+      <c r="A137" s="3">
+        <v>175</v>
       </c>
       <c r="B137" t="s">
         <v>12</v>
@@ -3819,7 +3847,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B138" t="s">
         <v>12</v>
@@ -3830,7 +3858,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B139" t="s">
         <v>12</v>
@@ -3841,7 +3869,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B140" t="s">
         <v>12</v>
@@ -3851,8 +3879,8 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A141" s="3">
-        <v>182</v>
+      <c r="A141">
+        <v>181</v>
       </c>
       <c r="B141" t="s">
         <v>12</v>
@@ -3862,8 +3890,8 @@
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142">
-        <v>184</v>
+      <c r="A142" s="3">
+        <v>182</v>
       </c>
       <c r="B142" t="s">
         <v>12</v>
@@ -3874,7 +3902,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B143" t="s">
         <v>12</v>
@@ -3884,8 +3912,8 @@
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A144" s="3">
-        <v>191</v>
+      <c r="A144">
+        <v>189</v>
       </c>
       <c r="B144" t="s">
         <v>12</v>
@@ -3895,8 +3923,8 @@
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145">
-        <v>193</v>
+      <c r="A145" s="3">
+        <v>191</v>
       </c>
       <c r="B145" t="s">
         <v>12</v>
@@ -3907,7 +3935,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B146" t="s">
         <v>12</v>
@@ -3918,7 +3946,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B147" t="s">
         <v>12</v>
@@ -3929,7 +3957,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B148" t="s">
         <v>12</v>
@@ -3940,7 +3968,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B149" t="s">
         <v>12</v>
@@ -3950,8 +3978,8 @@
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A150" s="3">
-        <v>198</v>
+      <c r="A150">
+        <v>197</v>
       </c>
       <c r="B150" t="s">
         <v>12</v>
@@ -3962,7 +3990,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B151" t="s">
         <v>12</v>
@@ -3972,8 +4000,8 @@
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A152">
-        <v>200</v>
+      <c r="A152" s="3">
+        <v>199</v>
       </c>
       <c r="B152" t="s">
         <v>12</v>
@@ -3984,7 +4012,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B153" t="s">
         <v>12</v>
@@ -3995,7 +4023,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B154" t="s">
         <v>12</v>
@@ -4006,7 +4034,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B155" t="s">
         <v>12</v>
@@ -4017,7 +4045,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B156" t="s">
         <v>12</v>
@@ -4028,7 +4056,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B157" t="s">
         <v>12</v>
@@ -4039,7 +4067,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B158" t="s">
         <v>12</v>
@@ -4050,7 +4078,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B159" t="s">
         <v>12</v>
@@ -4061,7 +4089,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B160" t="s">
         <v>12</v>
@@ -4071,8 +4099,8 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" s="3">
-        <v>215</v>
+      <c r="A161">
+        <v>214</v>
       </c>
       <c r="B161" t="s">
         <v>12</v>
@@ -4083,7 +4111,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B162" t="s">
         <v>12</v>
@@ -4093,8 +4121,8 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163">
-        <v>219</v>
+      <c r="A163" s="3">
+        <v>216</v>
       </c>
       <c r="B163" t="s">
         <v>12</v>
@@ -4105,7 +4133,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B164" t="s">
         <v>12</v>
@@ -4115,8 +4143,8 @@
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" s="3">
-        <v>224</v>
+      <c r="A165">
+        <v>221</v>
       </c>
       <c r="B165" t="s">
         <v>12</v>
@@ -4126,8 +4154,8 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166">
-        <v>225</v>
+      <c r="A166" s="3">
+        <v>224</v>
       </c>
       <c r="B166" t="s">
         <v>12</v>
@@ -4138,7 +4166,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B167" t="s">
         <v>12</v>
@@ -4149,7 +4177,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B168" t="s">
         <v>12</v>
@@ -4160,7 +4188,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B169" t="s">
         <v>12</v>
@@ -4170,8 +4198,8 @@
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A170" s="3">
-        <v>231</v>
+      <c r="A170">
+        <v>230</v>
       </c>
       <c r="B170" t="s">
         <v>12</v>
@@ -4182,7 +4210,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B171" t="s">
         <v>12</v>
@@ -4192,8 +4220,8 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172">
-        <v>233</v>
+      <c r="A172" s="3">
+        <v>232</v>
       </c>
       <c r="B172" t="s">
         <v>12</v>
@@ -4204,7 +4232,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B173" t="s">
         <v>12</v>
@@ -4215,7 +4243,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B174" t="s">
         <v>12</v>
@@ -4225,8 +4253,8 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" s="3">
-        <v>239</v>
+      <c r="A175">
+        <v>238</v>
       </c>
       <c r="B175" t="s">
         <v>12</v>
@@ -4236,8 +4264,8 @@
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176">
-        <v>546</v>
+      <c r="A176" s="3">
+        <v>239</v>
       </c>
       <c r="B176" t="s">
         <v>12</v>
@@ -4247,8 +4275,8 @@
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="3">
-        <v>584</v>
+      <c r="A177">
+        <v>546</v>
       </c>
       <c r="B177" t="s">
         <v>12</v>
@@ -4259,7 +4287,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="3">
-        <v>600</v>
+        <v>584</v>
       </c>
       <c r="B178" t="s">
         <v>12</v>
@@ -4269,8 +4297,8 @@
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179">
-        <v>630</v>
+      <c r="A179" s="3">
+        <v>600</v>
       </c>
       <c r="B179" t="s">
         <v>12</v>
@@ -4281,7 +4309,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="B180" t="s">
         <v>12</v>
@@ -4292,7 +4320,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B181" t="s">
         <v>12</v>
@@ -4303,7 +4331,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B182" t="s">
         <v>12</v>
@@ -4314,7 +4342,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183">
-        <v>718</v>
+        <v>643</v>
       </c>
       <c r="B183" t="s">
         <v>12</v>
@@ -4325,7 +4353,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184">
-        <v>763</v>
+        <v>718</v>
       </c>
       <c r="B184" t="s">
         <v>12</v>
@@ -4335,8 +4363,8 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" s="3">
-        <v>782</v>
+      <c r="A185">
+        <v>763</v>
       </c>
       <c r="B185" t="s">
         <v>12</v>
@@ -4347,7 +4375,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
-        <v>846</v>
+        <v>782</v>
       </c>
       <c r="B186" t="s">
         <v>12</v>
@@ -4357,8 +4385,8 @@
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A187">
-        <v>852</v>
+      <c r="A187" s="3">
+        <v>846</v>
       </c>
       <c r="B187" t="s">
         <v>12</v>
@@ -4369,7 +4397,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188">
-        <v>869</v>
+        <v>852</v>
       </c>
       <c r="B188" t="s">
         <v>12</v>
@@ -4380,18 +4408,18 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189">
-        <v>610</v>
+        <v>869</v>
       </c>
       <c r="B189" t="s">
         <v>12</v>
       </c>
       <c r="C189" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190">
-        <v>784</v>
+        <v>610</v>
       </c>
       <c r="B190" t="s">
         <v>12</v>
@@ -4402,18 +4430,18 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191">
-        <v>684</v>
+        <v>784</v>
       </c>
       <c r="B191" t="s">
         <v>12</v>
       </c>
       <c r="C191" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192">
-        <v>787</v>
+        <v>684</v>
       </c>
       <c r="B192" t="s">
         <v>12</v>
@@ -4424,29 +4452,29 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193">
-        <v>54</v>
+        <v>787</v>
       </c>
       <c r="B193" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="C193" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A194" s="3">
-        <v>101</v>
+      <c r="A194">
+        <v>3942</v>
       </c>
       <c r="B194" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="C194" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="B195" t="s">
         <v>75</v>
@@ -4457,7 +4485,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="3">
-        <v>240</v>
+        <v>101</v>
       </c>
       <c r="B196" t="s">
         <v>75</v>
@@ -4468,7 +4496,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197">
-        <v>698</v>
+        <v>106</v>
       </c>
       <c r="B197" t="s">
         <v>75</v>
@@ -4478,8 +4506,8 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A198" s="4">
-        <v>703</v>
+      <c r="A198" s="3">
+        <v>240</v>
       </c>
       <c r="B198" t="s">
         <v>75</v>
@@ -4490,7 +4518,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199">
-        <v>788</v>
+        <v>698</v>
       </c>
       <c r="B199" t="s">
         <v>75</v>
@@ -4501,7 +4529,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="4">
-        <v>845</v>
+        <v>703</v>
       </c>
       <c r="B200" t="s">
         <v>75</v>
@@ -4512,29 +4540,29 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201">
-        <v>61</v>
+        <v>788</v>
       </c>
       <c r="B201" t="s">
         <v>75</v>
       </c>
       <c r="C201" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A202">
-        <v>102</v>
+      <c r="A202" s="4">
+        <v>845</v>
       </c>
       <c r="B202" t="s">
         <v>75</v>
       </c>
       <c r="C202" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="B203" t="s">
         <v>75</v>
@@ -4545,7 +4573,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B204" t="s">
         <v>75</v>
@@ -4555,53 +4583,47 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A205" s="3">
-        <v>134</v>
+      <c r="A205">
+        <v>103</v>
       </c>
       <c r="B205" t="s">
         <v>75</v>
       </c>
       <c r="C205" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206">
-        <v>422</v>
+        <v>104</v>
       </c>
       <c r="B206" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C206" t="s">
-        <v>76</v>
-      </c>
-      <c r="D206" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A207">
-        <v>423</v>
+      <c r="A207" s="3">
+        <v>134</v>
       </c>
       <c r="B207" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C207" t="s">
-        <v>76</v>
-      </c>
-      <c r="D207" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B208" t="s">
         <v>79</v>
       </c>
       <c r="C208" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D208" t="s">
         <v>77</v>
@@ -4609,112 +4631,118 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209">
-        <v>1751</v>
+        <v>423</v>
       </c>
       <c r="B209" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C209" t="s">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="D209" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210">
-        <v>1752</v>
+        <v>424</v>
       </c>
       <c r="B210" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C210" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="D210" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211">
-        <v>908</v>
+        <v>1751</v>
       </c>
       <c r="B211" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="C211" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212">
-        <v>909</v>
+        <v>1752</v>
       </c>
       <c r="B212" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="C212" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213">
-        <v>318</v>
+        <v>908</v>
       </c>
       <c r="B213" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C213" t="s">
-        <v>22</v>
-      </c>
-      <c r="D213" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214">
-        <v>319</v>
+        <v>909</v>
       </c>
       <c r="B214" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C214" t="s">
-        <v>22</v>
-      </c>
-      <c r="D214" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215">
-        <v>794</v>
+        <v>318</v>
       </c>
       <c r="B215" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C215" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="D215" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A216" s="3">
-        <v>11</v>
+      <c r="A216">
+        <v>319</v>
       </c>
       <c r="B216" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C216" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="D216" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217">
-        <v>48</v>
+        <v>794</v>
       </c>
       <c r="B217" t="s">
         <v>24</v>
       </c>
       <c r="C217" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A218">
-        <v>599</v>
+      <c r="A218" s="3">
+        <v>11</v>
       </c>
       <c r="B218" t="s">
         <v>24</v>
@@ -4724,8 +4752,8 @@
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A219" s="3">
-        <v>708</v>
+      <c r="A219">
+        <v>48</v>
       </c>
       <c r="B219" t="s">
         <v>24</v>
@@ -4736,7 +4764,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220">
-        <v>750</v>
+        <v>599</v>
       </c>
       <c r="B220" t="s">
         <v>24</v>
@@ -4747,7 +4775,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
-        <v>864</v>
+        <v>708</v>
       </c>
       <c r="B221" t="s">
         <v>24</v>
@@ -4758,40 +4786,40 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222">
-        <v>571</v>
+        <v>750</v>
       </c>
       <c r="B222" t="s">
         <v>24</v>
       </c>
       <c r="C222" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A223">
-        <v>595</v>
+      <c r="A223" s="3">
+        <v>864</v>
       </c>
       <c r="B223" t="s">
         <v>24</v>
       </c>
       <c r="C223" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224">
-        <v>598</v>
+        <v>571</v>
       </c>
       <c r="B224" t="s">
         <v>24</v>
       </c>
       <c r="C224" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="B225" t="s">
         <v>24</v>
@@ -4802,7 +4830,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226">
-        <v>668</v>
+        <v>598</v>
       </c>
       <c r="B226" t="s">
         <v>24</v>
@@ -4812,8 +4840,8 @@
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A227" s="3">
-        <v>675</v>
+      <c r="A227">
+        <v>602</v>
       </c>
       <c r="B227" t="s">
         <v>24</v>
@@ -4824,7 +4852,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228">
-        <v>692</v>
+        <v>668</v>
       </c>
       <c r="B228" t="s">
         <v>24</v>
@@ -4835,7 +4863,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="3">
-        <v>699</v>
+        <v>675</v>
       </c>
       <c r="B229" t="s">
         <v>24</v>
@@ -4845,8 +4873,8 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A230" s="3">
-        <v>716</v>
+      <c r="A230">
+        <v>692</v>
       </c>
       <c r="B230" t="s">
         <v>24</v>
@@ -4857,7 +4885,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
-        <v>764</v>
+        <v>699</v>
       </c>
       <c r="B231" t="s">
         <v>24</v>
@@ -4867,8 +4895,8 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A232">
-        <v>767</v>
+      <c r="A232" s="3">
+        <v>716</v>
       </c>
       <c r="B232" t="s">
         <v>24</v>
@@ -4879,7 +4907,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="3">
-        <v>790</v>
+        <v>764</v>
       </c>
       <c r="B233" t="s">
         <v>24</v>
@@ -4890,7 +4918,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234">
-        <v>837</v>
+        <v>767</v>
       </c>
       <c r="B234" t="s">
         <v>24</v>
@@ -4901,154 +4929,145 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="3">
-        <v>768</v>
+        <v>790</v>
       </c>
       <c r="B235" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C235" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236">
-        <v>69</v>
+        <v>837</v>
       </c>
       <c r="B236" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C236" t="s">
-        <v>32</v>
-      </c>
-      <c r="D236" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="3">
-        <v>283</v>
+        <v>768</v>
       </c>
       <c r="B237" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C237" t="s">
-        <v>32</v>
-      </c>
-      <c r="D237" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238">
-        <v>646</v>
+        <v>69</v>
       </c>
       <c r="B238" t="s">
         <v>31</v>
       </c>
       <c r="C238" t="s">
+        <v>32</v>
+      </c>
+      <c r="D238" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="3">
+        <v>283</v>
+      </c>
+      <c r="B239" t="s">
+        <v>31</v>
+      </c>
+      <c r="C239" t="s">
+        <v>32</v>
+      </c>
+      <c r="D239" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>646</v>
+      </c>
+      <c r="B240" t="s">
+        <v>31</v>
+      </c>
+      <c r="C240" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239">
-        <v>650</v>
-      </c>
-      <c r="B239" t="s">
-        <v>35</v>
-      </c>
-      <c r="C239" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A240" s="3">
-        <v>570</v>
-      </c>
-      <c r="B240" t="s">
-        <v>36</v>
-      </c>
-      <c r="C240" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241">
-        <v>822</v>
+        <v>650</v>
       </c>
       <c r="B241" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C241" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="3">
-        <v>13</v>
+        <v>570</v>
       </c>
       <c r="B242" t="s">
         <v>36</v>
       </c>
       <c r="C242" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243">
-        <v>774</v>
+        <v>822</v>
       </c>
       <c r="B243" t="s">
         <v>36</v>
       </c>
       <c r="C243" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" s="3">
+        <v>13</v>
+      </c>
+      <c r="B244" t="s">
+        <v>36</v>
+      </c>
+      <c r="C244" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A244">
-        <v>237</v>
-      </c>
-      <c r="B244" t="s">
-        <v>40</v>
-      </c>
-      <c r="C244" t="s">
-        <v>41</v>
-      </c>
-      <c r="D244" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A245" s="3">
-        <v>322</v>
+      <c r="A245">
+        <v>774</v>
       </c>
       <c r="B245" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C245" t="s">
-        <v>41</v>
-      </c>
-      <c r="D245" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A246">
-        <v>323</v>
+      <c r="A246" s="3">
+        <v>3954</v>
       </c>
       <c r="B246" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C246" t="s">
-        <v>41</v>
-      </c>
-      <c r="D246" t="s">
-        <v>42</v>
+        <v>590</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247">
-        <v>324</v>
+        <v>237</v>
       </c>
       <c r="B247" t="s">
         <v>40</v>
@@ -5061,8 +5080,8 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A248">
-        <v>566</v>
+      <c r="A248" s="3">
+        <v>322</v>
       </c>
       <c r="B248" t="s">
         <v>40</v>
@@ -5071,12 +5090,12 @@
         <v>41</v>
       </c>
       <c r="D248" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249">
-        <v>915</v>
+        <v>323</v>
       </c>
       <c r="B249" t="s">
         <v>40</v>
@@ -5084,10 +5103,13 @@
       <c r="C249" t="s">
         <v>41</v>
       </c>
+      <c r="D249" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250">
-        <v>916</v>
+        <v>324</v>
       </c>
       <c r="B250" t="s">
         <v>40</v>
@@ -5095,10 +5117,13 @@
       <c r="C250" t="s">
         <v>41</v>
       </c>
+      <c r="D250" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251">
-        <v>917</v>
+        <v>566</v>
       </c>
       <c r="B251" t="s">
         <v>40</v>
@@ -5106,76 +5131,79 @@
       <c r="C251" t="s">
         <v>41</v>
       </c>
+      <c r="D251" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252">
-        <v>378</v>
+        <v>915</v>
       </c>
       <c r="B252" t="s">
-        <v>44</v>
-      </c>
-      <c r="C252" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="C252" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253">
-        <v>898</v>
+        <v>916</v>
       </c>
       <c r="B253" t="s">
-        <v>44</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="C253" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254">
-        <v>899</v>
+        <v>917</v>
       </c>
       <c r="B254" t="s">
-        <v>44</v>
-      </c>
-      <c r="C254" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="C254" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255">
-        <v>70</v>
+        <v>378</v>
       </c>
       <c r="B255" t="s">
         <v>44</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256">
-        <v>894</v>
+        <v>898</v>
       </c>
       <c r="B256" t="s">
         <v>44</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A257" s="3">
-        <v>895</v>
+      <c r="A257">
+        <v>899</v>
       </c>
       <c r="B257" t="s">
         <v>44</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A258" s="3">
-        <v>896</v>
+      <c r="A258">
+        <v>70</v>
       </c>
       <c r="B258" t="s">
         <v>44</v>
@@ -5186,7 +5214,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="B259" t="s">
         <v>44</v>
@@ -5196,107 +5224,107 @@
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A260">
-        <v>900</v>
+      <c r="A260" s="3">
+        <v>895</v>
       </c>
       <c r="B260" t="s">
         <v>44</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A261">
-        <v>243</v>
+      <c r="A261" s="3">
+        <v>896</v>
       </c>
       <c r="B261" t="s">
-        <v>48</v>
-      </c>
-      <c r="C261" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262">
-        <v>244</v>
+        <v>897</v>
       </c>
       <c r="B262" t="s">
-        <v>48</v>
-      </c>
-      <c r="C262" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263">
-        <v>679</v>
+        <v>900</v>
       </c>
       <c r="B263" t="s">
-        <v>48</v>
-      </c>
-      <c r="C263" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264">
-        <v>401</v>
+        <v>243</v>
       </c>
       <c r="B264" t="s">
         <v>48</v>
       </c>
       <c r="C264" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265">
-        <v>713</v>
+        <v>244</v>
       </c>
       <c r="B265" t="s">
         <v>48</v>
       </c>
       <c r="C265" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266">
-        <v>993</v>
+        <v>679</v>
       </c>
       <c r="B266" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C266" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A267" s="3">
-        <v>994</v>
+      <c r="A267">
+        <v>401</v>
       </c>
       <c r="B267" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C267" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A268" s="3">
-        <v>995</v>
+      <c r="A268">
+        <v>713</v>
       </c>
       <c r="B268" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C268" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="B269" t="s">
         <v>53</v>
@@ -5306,8 +5334,8 @@
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A270">
-        <v>997</v>
+      <c r="A270" s="3">
+        <v>994</v>
       </c>
       <c r="B270" t="s">
         <v>53</v>
@@ -5317,8 +5345,8 @@
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A271">
-        <v>998</v>
+      <c r="A271" s="3">
+        <v>995</v>
       </c>
       <c r="B271" t="s">
         <v>53</v>
@@ -5329,7 +5357,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="B272" t="s">
         <v>53</v>
@@ -5340,7 +5368,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="B273" t="s">
         <v>53</v>
@@ -5351,7 +5379,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="B274" t="s">
         <v>53</v>
@@ -5361,8 +5389,8 @@
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A275" s="3">
-        <v>1002</v>
+      <c r="A275">
+        <v>999</v>
       </c>
       <c r="B275" t="s">
         <v>53</v>
@@ -5372,8 +5400,8 @@
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A276" s="3">
-        <v>1003</v>
+      <c r="A276">
+        <v>1000</v>
       </c>
       <c r="B276" t="s">
         <v>53</v>
@@ -5384,7 +5412,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="B277" t="s">
         <v>53</v>
@@ -5394,8 +5422,8 @@
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A278">
-        <v>1005</v>
+      <c r="A278" s="3">
+        <v>1002</v>
       </c>
       <c r="B278" t="s">
         <v>53</v>
@@ -5405,8 +5433,8 @@
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A279">
-        <v>1006</v>
+      <c r="A279" s="3">
+        <v>1003</v>
       </c>
       <c r="B279" t="s">
         <v>53</v>
@@ -5417,7 +5445,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="B280" t="s">
         <v>53</v>
@@ -5428,40 +5456,40 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281">
-        <v>301</v>
+        <v>1005</v>
       </c>
       <c r="B281" t="s">
         <v>53</v>
       </c>
       <c r="C281" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282">
-        <v>989</v>
+        <v>1006</v>
       </c>
       <c r="B282" t="s">
         <v>53</v>
       </c>
       <c r="C282" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283">
-        <v>990</v>
+        <v>1007</v>
       </c>
       <c r="B283" t="s">
         <v>53</v>
       </c>
       <c r="C283" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284">
-        <v>991</v>
+        <v>301</v>
       </c>
       <c r="B284" t="s">
         <v>53</v>
@@ -5472,7 +5500,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="B285" t="s">
         <v>53</v>
@@ -5483,137 +5511,128 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286">
-        <v>1566</v>
+        <v>990</v>
       </c>
       <c r="B286" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C286" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287">
-        <v>1138</v>
+        <v>991</v>
       </c>
       <c r="B287" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C287" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288">
-        <v>1139</v>
+        <v>992</v>
       </c>
       <c r="B288" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C288" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289">
-        <v>1135</v>
+        <v>1566</v>
       </c>
       <c r="B289" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C289" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="B290" t="s">
         <v>59</v>
       </c>
       <c r="C290" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291">
-        <v>316</v>
+        <v>1139</v>
       </c>
       <c r="B291" t="s">
         <v>59</v>
       </c>
       <c r="C291" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292">
-        <v>373</v>
+        <v>1135</v>
       </c>
       <c r="B292" t="s">
         <v>59</v>
       </c>
       <c r="C292" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B293" t="s">
         <v>59</v>
       </c>
       <c r="C293" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294">
-        <v>74</v>
+        <v>316</v>
       </c>
       <c r="B294" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C294" t="s">
-        <v>83</v>
-      </c>
-      <c r="D294" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295">
-        <v>325</v>
+        <v>373</v>
       </c>
       <c r="B295" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C295" t="s">
-        <v>83</v>
-      </c>
-      <c r="D295" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296">
-        <v>326</v>
+        <v>1137</v>
       </c>
       <c r="B296" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C296" t="s">
-        <v>83</v>
-      </c>
-      <c r="D296" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297">
-        <v>327</v>
+        <v>74</v>
       </c>
       <c r="B297" t="s">
         <v>85</v>
@@ -5627,40 +5646,49 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298">
-        <v>156</v>
+        <v>325</v>
       </c>
       <c r="B298" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C298" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="D298" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299">
-        <v>635</v>
+        <v>326</v>
       </c>
       <c r="B299" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C299" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="D299" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A300" s="3">
-        <v>667</v>
+      <c r="A300">
+        <v>327</v>
       </c>
       <c r="B300" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C300" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="D300" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301">
-        <v>730</v>
+        <v>156</v>
       </c>
       <c r="B301" t="s">
         <v>62</v>
@@ -5671,353 +5699,353 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302">
-        <v>277</v>
+        <v>635</v>
       </c>
       <c r="B302" t="s">
         <v>62</v>
       </c>
       <c r="C302" t="s">
-        <v>60</v>
-      </c>
-      <c r="D302" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A303">
-        <v>1877</v>
+      <c r="A303" s="3">
+        <v>667</v>
       </c>
       <c r="B303" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C303" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304">
-        <v>1878</v>
+        <v>730</v>
       </c>
       <c r="B304" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C304" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A305" s="3">
-        <v>1879</v>
+      <c r="A305">
+        <v>277</v>
       </c>
       <c r="B305" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C305" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="D305" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306">
-        <v>1029</v>
+        <v>1877</v>
       </c>
       <c r="B306" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C306" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307">
-        <v>265</v>
+        <v>1878</v>
       </c>
       <c r="B307" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C307" t="s">
-        <v>68</v>
-      </c>
-      <c r="D307" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A308">
-        <v>36</v>
+      <c r="A308" s="3">
+        <v>1879</v>
       </c>
       <c r="B308" t="s">
-        <v>252</v>
+        <v>64</v>
       </c>
       <c r="C308" t="s">
-        <v>253</v>
-      </c>
-      <c r="D308" t="s">
-        <v>254</v>
+        <v>63</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309">
-        <v>73</v>
+        <v>1029</v>
       </c>
       <c r="B309" t="s">
-        <v>255</v>
+        <v>66</v>
       </c>
       <c r="C309" t="s">
-        <v>257</v>
-      </c>
-      <c r="D309" t="s">
-        <v>256</v>
+        <v>65</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310">
-        <v>1733</v>
+        <v>265</v>
       </c>
       <c r="B310" t="s">
-        <v>255</v>
+        <v>69</v>
       </c>
       <c r="C310" t="s">
-        <v>258</v>
+        <v>68</v>
+      </c>
+      <c r="D310" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311">
-        <v>1734</v>
+        <v>36</v>
       </c>
       <c r="B311" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C311" t="s">
-        <v>259</v>
+        <v>253</v>
+      </c>
+      <c r="D311" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312">
-        <v>158</v>
+        <v>73</v>
       </c>
       <c r="B312" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C312" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D312" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313">
-        <v>227</v>
+        <v>1733</v>
       </c>
       <c r="B313" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C313" t="s">
-        <v>264</v>
-      </c>
-      <c r="D313" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314">
-        <v>1201</v>
+        <v>1734</v>
       </c>
       <c r="B314" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C314" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315">
+        <v>158</v>
+      </c>
+      <c r="B315" t="s">
+        <v>262</v>
+      </c>
+      <c r="C315" t="s">
+        <v>261</v>
+      </c>
+      <c r="D315" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>227</v>
+      </c>
+      <c r="B316" t="s">
+        <v>265</v>
+      </c>
+      <c r="C316" t="s">
+        <v>264</v>
+      </c>
+      <c r="D316" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>1201</v>
+      </c>
+      <c r="B317" t="s">
+        <v>265</v>
+      </c>
+      <c r="C317" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A318">
         <v>252</v>
       </c>
-      <c r="B315" t="s">
+      <c r="B318" t="s">
         <v>266</v>
       </c>
-      <c r="C315" t="s">
+      <c r="C318" t="s">
         <v>268</v>
       </c>
-      <c r="D315" t="s">
+      <c r="D318" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A319" t="s">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A320">
-        <v>32</v>
-      </c>
-      <c r="B320" t="s">
-        <v>36</v>
-      </c>
-      <c r="C320" s="15" t="s">
-        <v>558</v>
-      </c>
-      <c r="D320" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A321">
-        <v>79</v>
-      </c>
-      <c r="B321" t="s">
-        <v>36</v>
-      </c>
-      <c r="C321" s="15" t="s">
-        <v>565</v>
-      </c>
-      <c r="D321" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A322">
-        <v>142</v>
-      </c>
-      <c r="B322" t="s">
-        <v>36</v>
-      </c>
-      <c r="C322" s="15" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323">
-        <v>198</v>
+        <v>32</v>
       </c>
       <c r="B323" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C323" s="15" t="s">
-        <v>568</v>
+        <v>558</v>
+      </c>
+      <c r="D323" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324">
-        <v>199</v>
+        <v>79</v>
       </c>
       <c r="B324" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C324" s="15" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D324" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="B325" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C325" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="D325" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="B326" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C326" s="15" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="B327" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C327" s="15" t="s">
-        <v>570</v>
+        <v>568</v>
+      </c>
+      <c r="D327" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328">
-        <v>275</v>
+        <v>200</v>
       </c>
       <c r="B328" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C328" s="15" t="s">
-        <v>49</v>
+        <v>568</v>
+      </c>
+      <c r="D328" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="B329" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C329" s="15" t="s">
-        <v>49</v>
+        <v>570</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B330" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C330" s="15" t="s">
-        <v>518</v>
+        <v>570</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A331">
-        <v>443</v>
+        <v>275</v>
       </c>
       <c r="B331" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C331" s="15" t="s">
-        <v>559</v>
+        <v>49</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A332">
-        <v>444</v>
+        <v>276</v>
       </c>
       <c r="B332" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C332" s="15" t="s">
-        <v>559</v>
+        <v>49</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A333">
-        <v>445</v>
+        <v>232</v>
       </c>
       <c r="B333" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C333" s="15" t="s">
-        <v>559</v>
+        <v>518</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A334">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B334" t="s">
         <v>0</v>
@@ -6028,7 +6056,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A335">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B335" t="s">
         <v>0</v>
@@ -6039,7 +6067,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A336">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B336" t="s">
         <v>0</v>
@@ -6050,7 +6078,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A337">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B337" t="s">
         <v>0</v>
@@ -6061,7 +6089,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B338" t="s">
         <v>0</v>
@@ -6069,13 +6097,10 @@
       <c r="C338" s="15" t="s">
         <v>559</v>
       </c>
-      <c r="D338" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A339">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B339" t="s">
         <v>0</v>
@@ -6083,46 +6108,49 @@
       <c r="C339" s="15" t="s">
         <v>559</v>
       </c>
-      <c r="D339" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A340">
-        <v>206</v>
+        <v>449</v>
       </c>
       <c r="B340" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C340" s="15" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A341">
-        <v>207</v>
+        <v>450</v>
       </c>
       <c r="B341" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C341" s="15" t="s">
-        <v>560</v>
+        <v>559</v>
+      </c>
+      <c r="D341" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A342">
-        <v>208</v>
+        <v>451</v>
       </c>
       <c r="B342" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C342" s="15" t="s">
-        <v>560</v>
+        <v>559</v>
+      </c>
+      <c r="D342" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A343">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B343" t="s">
         <v>5</v>
@@ -6133,7 +6161,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A344">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B344" t="s">
         <v>5</v>
@@ -6144,7 +6172,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A345">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B345" t="s">
         <v>5</v>
@@ -6155,7 +6183,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A346">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B346" t="s">
         <v>5</v>
@@ -6163,13 +6191,10 @@
       <c r="C346" s="15" t="s">
         <v>560</v>
       </c>
-      <c r="D346" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B347" t="s">
         <v>5</v>
@@ -6180,7 +6205,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B348" t="s">
         <v>5</v>
@@ -6191,7 +6216,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A349">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B349" t="s">
         <v>5</v>
@@ -6199,10 +6224,13 @@
       <c r="C349" s="15" t="s">
         <v>560</v>
       </c>
+      <c r="D349" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B350" t="s">
         <v>5</v>
@@ -6213,7 +6241,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A351">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B351" t="s">
         <v>5</v>
@@ -6224,7 +6252,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B352" t="s">
         <v>5</v>
@@ -6235,7 +6263,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B353" t="s">
         <v>5</v>
@@ -6246,7 +6274,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B354" t="s">
         <v>5</v>
@@ -6257,7 +6285,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B355" t="s">
         <v>5</v>
@@ -6268,7 +6296,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B356" t="s">
         <v>5</v>
@@ -6276,13 +6304,10 @@
       <c r="C356" s="15" t="s">
         <v>560</v>
       </c>
-      <c r="D356" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B357" t="s">
         <v>5</v>
@@ -6290,57 +6315,60 @@
       <c r="C357" s="15" t="s">
         <v>560</v>
       </c>
-      <c r="D357" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358">
-        <v>69</v>
+        <v>221</v>
       </c>
       <c r="B358" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C358" s="15" t="s">
-        <v>17</v>
+        <v>560</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359">
-        <v>70</v>
+        <v>222</v>
       </c>
       <c r="B359" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C359" s="15" t="s">
-        <v>17</v>
+        <v>560</v>
+      </c>
+      <c r="D359" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360">
-        <v>71</v>
+        <v>223</v>
       </c>
       <c r="B360" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C360" s="15" t="s">
-        <v>17</v>
+        <v>560</v>
+      </c>
+      <c r="D360" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361">
-        <v>72</v>
+        <v>3943</v>
       </c>
       <c r="B361" t="s">
-        <v>12</v>
-      </c>
-      <c r="C361" s="15" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="C361" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B362" t="s">
         <v>12</v>
@@ -6351,7 +6379,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B363" t="s">
         <v>12</v>
@@ -6362,7 +6390,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B364" t="s">
         <v>12</v>
@@ -6373,7 +6401,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B365" t="s">
         <v>12</v>
@@ -6384,7 +6412,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B366" t="s">
         <v>12</v>
@@ -6395,7 +6423,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B367" t="s">
         <v>12</v>
@@ -6406,112 +6434,112 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B368" t="s">
         <v>12</v>
       </c>
       <c r="C368" s="15" t="s">
-        <v>561</v>
+        <v>17</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A369">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B369" t="s">
         <v>12</v>
       </c>
-      <c r="C369" s="21" t="s">
+      <c r="C369" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A370">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B370" t="s">
         <v>12</v>
       </c>
-      <c r="C370" s="21" t="s">
+      <c r="C370" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A371">
-        <v>417</v>
+        <v>78</v>
       </c>
       <c r="B371" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="C371" s="15" t="s">
-        <v>562</v>
-      </c>
-      <c r="D371" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A372">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B372" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C372" s="15" t="s">
-        <v>563</v>
-      </c>
-      <c r="D372" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A373">
-        <v>277</v>
+        <v>83</v>
       </c>
       <c r="B373" t="s">
-        <v>53</v>
-      </c>
-      <c r="C373" s="15" t="s">
-        <v>571</v>
+        <v>12</v>
+      </c>
+      <c r="C373" s="21" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A374">
-        <v>278</v>
+        <v>84</v>
       </c>
       <c r="B374" t="s">
-        <v>53</v>
-      </c>
-      <c r="C374" s="15" t="s">
-        <v>571</v>
+        <v>12</v>
+      </c>
+      <c r="C374" s="21" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A375">
-        <v>279</v>
+        <v>417</v>
       </c>
       <c r="B375" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="C375" s="15" t="s">
-        <v>571</v>
+        <v>562</v>
+      </c>
+      <c r="D375" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A376">
-        <v>280</v>
+        <v>81</v>
       </c>
       <c r="B376" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C376" s="15" t="s">
-        <v>571</v>
+        <v>563</v>
+      </c>
+      <c r="D376" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A377">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B377" t="s">
         <v>53</v>
@@ -6522,7 +6550,7 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A378">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B378" t="s">
         <v>53</v>
@@ -6533,7 +6561,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A379">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B379" t="s">
         <v>53</v>
@@ -6544,172 +6572,304 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A380">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B380" t="s">
         <v>53</v>
       </c>
       <c r="C380" s="15" t="s">
-        <v>52</v>
+        <v>571</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A381">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B381" t="s">
         <v>53</v>
       </c>
       <c r="C381" s="15" t="s">
-        <v>52</v>
+        <v>571</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A382">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B382" t="s">
         <v>53</v>
       </c>
       <c r="C382" s="15" t="s">
-        <v>52</v>
+        <v>571</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A383">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B383" t="s">
         <v>53</v>
       </c>
       <c r="C383" s="15" t="s">
-        <v>52</v>
+        <v>571</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A384">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B384" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C384" s="15" t="s">
-        <v>572</v>
+        <v>52</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A385">
-        <v>322</v>
+        <v>285</v>
       </c>
       <c r="B385" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="C385" s="15" t="s">
-        <v>573</v>
+        <v>52</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386">
-        <v>18</v>
+        <v>286</v>
       </c>
       <c r="B386" t="s">
-        <v>252</v>
+        <v>53</v>
       </c>
       <c r="C386" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="D386" t="s">
-        <v>254</v>
+        <v>52</v>
       </c>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A387">
-        <v>113</v>
+        <v>287</v>
       </c>
       <c r="B387" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C387" s="15" t="s">
-        <v>575</v>
+        <v>52</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A388">
-        <v>114</v>
+        <v>292</v>
       </c>
       <c r="B388" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="C388" s="15" t="s">
-        <v>576</v>
-      </c>
-      <c r="D388" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A389">
-        <v>401</v>
+        <v>322</v>
       </c>
       <c r="B389" t="s">
-        <v>75</v>
-      </c>
-      <c r="C389" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="D389" s="22" t="s">
-        <v>579</v>
+        <v>85</v>
+      </c>
+      <c r="C389" s="15" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A390">
-        <v>402</v>
+        <v>18</v>
       </c>
       <c r="B390" t="s">
-        <v>75</v>
-      </c>
-      <c r="C390" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="D390" s="22"/>
+        <v>252</v>
+      </c>
+      <c r="C390" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="D390" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A391">
-        <v>403</v>
+        <v>113</v>
       </c>
       <c r="B391" t="s">
-        <v>75</v>
-      </c>
-      <c r="C391" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="D391" s="22"/>
+        <v>24</v>
+      </c>
+      <c r="C391" s="15" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A392">
-        <v>404</v>
+        <v>114</v>
       </c>
       <c r="B392" t="s">
-        <v>75</v>
-      </c>
-      <c r="C392" s="22" t="s">
-        <v>578</v>
-      </c>
-      <c r="D392" s="22" t="s">
-        <v>579</v>
+        <v>24</v>
+      </c>
+      <c r="C392" s="15" t="s">
+        <v>576</v>
+      </c>
+      <c r="D392" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A393">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B393" t="s">
         <v>75</v>
       </c>
       <c r="C393" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D393" s="22" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <v>402</v>
+      </c>
+      <c r="B394" t="s">
+        <v>75</v>
+      </c>
+      <c r="C394" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D394" s="22"/>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <v>403</v>
+      </c>
+      <c r="B395" t="s">
+        <v>75</v>
+      </c>
+      <c r="C395" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D395" s="22"/>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <v>404</v>
+      </c>
+      <c r="B396" t="s">
+        <v>75</v>
+      </c>
+      <c r="C396" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D396" s="22" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A397">
+        <v>405</v>
+      </c>
+      <c r="B397" t="s">
+        <v>75</v>
+      </c>
+      <c r="C397" s="22" t="s">
         <v>580</v>
       </c>
-      <c r="D393" s="22"/>
+      <c r="D397" s="22"/>
+    </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A402" s="3">
+        <v>1421</v>
+      </c>
+      <c r="B402" t="s">
+        <v>586</v>
+      </c>
+      <c r="C402" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <v>1422</v>
+      </c>
+      <c r="B403" t="s">
+        <v>586</v>
+      </c>
+      <c r="C403" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <v>1423</v>
+      </c>
+      <c r="B404" t="s">
+        <v>586</v>
+      </c>
+      <c r="C404" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <v>1424</v>
+      </c>
+      <c r="B405" t="s">
+        <v>586</v>
+      </c>
+      <c r="C405" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <v>3520</v>
+      </c>
+      <c r="B406" t="s">
+        <v>586</v>
+      </c>
+      <c r="C406" s="23" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <v>3521</v>
+      </c>
+      <c r="B407" t="s">
+        <v>586</v>
+      </c>
+      <c r="C407" s="23" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <v>3946</v>
+      </c>
+      <c r="B408" t="s">
+        <v>586</v>
+      </c>
+      <c r="C408" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <v>3947</v>
+      </c>
+      <c r="B409" t="s">
+        <v>586</v>
+      </c>
+      <c r="C409" t="s">
+        <v>589</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7784,7 +7944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2D1DDA-4A02-0A44-A154-67090866577B}">
   <dimension ref="A1:C225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+    <sheetView topLeftCell="A185" workbookViewId="0">
       <selection activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new and updated csv's
</commit_message>
<xml_diff>
--- a/Data/Extra info verwijderde namen.xlsx
+++ b/Data/Extra info verwijderde namen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alielassche/Documents/GitHub/netwerk-huwelijksgedichten/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9290D42B-B445-9942-991F-C50E3D6698AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBE6911-F87E-A34E-B1EB-785142F107E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{91DC8FCD-999E-C04C-A5B7-D30830052C4B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{91DC8FCD-999E-C04C-A5B7-D30830052C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Drukkers" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="639">
   <si>
     <t>Goeree</t>
   </si>
@@ -1804,6 +1804,147 @@
   </si>
   <si>
     <t>Willem en David Goeree</t>
+  </si>
+  <si>
+    <t>Arnoldus Curtenius</t>
+  </si>
+  <si>
+    <t>Arnoldus (wed) Curtenius</t>
+  </si>
+  <si>
+    <t>Barent Visscher</t>
+  </si>
+  <si>
+    <t>Barent (wed) Visscher</t>
+  </si>
+  <si>
+    <t>Cornelis (II) Barlinckhof</t>
+  </si>
+  <si>
+    <t>Cornelis Barlinckhof</t>
+  </si>
+  <si>
+    <t>Gerrit Slaats</t>
+  </si>
+  <si>
+    <t>Gerrit (wed) Slaats</t>
+  </si>
+  <si>
+    <t>Harder van (wed) Ditmer</t>
+  </si>
+  <si>
+    <t>Harder van Ditmer</t>
+  </si>
+  <si>
+    <t>Hendrik van I (wed) Damme</t>
+  </si>
+  <si>
+    <t>Hendrik van (I) Damme</t>
+  </si>
+  <si>
+    <t>Hendrik van Damme</t>
+  </si>
+  <si>
+    <t>Hendrik van I Damme</t>
+  </si>
+  <si>
+    <t>Izaak van der I Vinne</t>
+  </si>
+  <si>
+    <t>Izaak van der II Vinne</t>
+  </si>
+  <si>
+    <t>Izaak van der Vinne</t>
+  </si>
+  <si>
+    <t>Isaak van der (I) Vinne</t>
+  </si>
+  <si>
+    <t>Jacobus Verheyde</t>
+  </si>
+  <si>
+    <t>Jacobus (I) Verheyde</t>
+  </si>
+  <si>
+    <t>Jan (I) Rieuwertsz</t>
+  </si>
+  <si>
+    <t>Jan (II) Rieuwertsz</t>
+  </si>
+  <si>
+    <t>Jan Rieuwertsz</t>
+  </si>
+  <si>
+    <t>Jan I Rieuwertsz</t>
+  </si>
+  <si>
+    <t>Jan II Rieuwertsz</t>
+  </si>
+  <si>
+    <t>Johannes van Oosterwyk</t>
+  </si>
+  <si>
+    <t>Joannes Oosterwyk</t>
+  </si>
+  <si>
+    <t>Matthijs (wed) Bastiaensz</t>
+  </si>
+  <si>
+    <t>Matthijs Bastiaensz</t>
+  </si>
+  <si>
+    <t>Michiel van I Leeuwen</t>
+  </si>
+  <si>
+    <t>Michiel van I (wed) Leeuwen</t>
+  </si>
+  <si>
+    <t>Michiel van II Leeuwen</t>
+  </si>
+  <si>
+    <t>Michiel van Leeuwen</t>
+  </si>
+  <si>
+    <t>Nicolaas (wed) Lobedanius</t>
+  </si>
+  <si>
+    <t>Nicolaus Lobedanius</t>
+  </si>
+  <si>
+    <t>Nicolaus (wed) Lobedanius</t>
+  </si>
+  <si>
+    <t>Nicolaas Lobedanius</t>
+  </si>
+  <si>
+    <t>Nicolaas (wed) Bos</t>
+  </si>
+  <si>
+    <t>Nicolaas Bos</t>
+  </si>
+  <si>
+    <t>Pieter I Muntendam</t>
+  </si>
+  <si>
+    <t>Pieter Muntendam</t>
+  </si>
+  <si>
+    <t>Pieter (I) Muntendam</t>
+  </si>
+  <si>
+    <t>Pieter (II) Muntendam</t>
+  </si>
+  <si>
+    <t>Porcevant (wed) Morgan</t>
+  </si>
+  <si>
+    <t>Porcevant Morgan</t>
+  </si>
+  <si>
+    <t>Reinier (erven) Leers</t>
+  </si>
+  <si>
+    <t>Reinier Leers</t>
   </si>
 </sst>
 </file>
@@ -2285,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC8214C-B4FA-7B44-AB5D-D8A034BCE402}">
-  <dimension ref="A1:D409"/>
+  <dimension ref="A1:D533"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A383" workbookViewId="0">
+      <selection activeCell="B401" sqref="B401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6869,6 +7010,1370 @@
       </c>
       <c r="C409" t="s">
         <v>589</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <v>428</v>
+      </c>
+      <c r="B410" t="s">
+        <v>592</v>
+      </c>
+      <c r="C410" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <v>642</v>
+      </c>
+      <c r="B411" t="s">
+        <v>592</v>
+      </c>
+      <c r="C411" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <v>3442</v>
+      </c>
+      <c r="B412" t="s">
+        <v>594</v>
+      </c>
+      <c r="C412" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <v>3443</v>
+      </c>
+      <c r="B413" t="s">
+        <v>594</v>
+      </c>
+      <c r="C413" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <v>356</v>
+      </c>
+      <c r="B414" t="s">
+        <v>594</v>
+      </c>
+      <c r="C414" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <v>1917</v>
+      </c>
+      <c r="B415" t="s">
+        <v>594</v>
+      </c>
+      <c r="C415" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <v>1918</v>
+      </c>
+      <c r="B416" t="s">
+        <v>594</v>
+      </c>
+      <c r="C416" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>1919</v>
+      </c>
+      <c r="B417" t="s">
+        <v>594</v>
+      </c>
+      <c r="C417" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A418" s="3">
+        <v>1920</v>
+      </c>
+      <c r="B418" t="s">
+        <v>594</v>
+      </c>
+      <c r="C418" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A419" s="3">
+        <v>1921</v>
+      </c>
+      <c r="B419" t="s">
+        <v>594</v>
+      </c>
+      <c r="C419" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>1922</v>
+      </c>
+      <c r="B420" t="s">
+        <v>594</v>
+      </c>
+      <c r="C420" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>1923</v>
+      </c>
+      <c r="B421" t="s">
+        <v>594</v>
+      </c>
+      <c r="C421" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>1924</v>
+      </c>
+      <c r="B422" t="s">
+        <v>594</v>
+      </c>
+      <c r="C422" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>1925</v>
+      </c>
+      <c r="B423" t="s">
+        <v>594</v>
+      </c>
+      <c r="C423" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>1926</v>
+      </c>
+      <c r="B424" t="s">
+        <v>594</v>
+      </c>
+      <c r="C424" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>1927</v>
+      </c>
+      <c r="B425" t="s">
+        <v>594</v>
+      </c>
+      <c r="C425" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>1928</v>
+      </c>
+      <c r="B426" t="s">
+        <v>594</v>
+      </c>
+      <c r="C426" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A427" s="3">
+        <v>1929</v>
+      </c>
+      <c r="B427" t="s">
+        <v>594</v>
+      </c>
+      <c r="C427" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>3458</v>
+      </c>
+      <c r="B428" t="s">
+        <v>597</v>
+      </c>
+      <c r="C428" s="23" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>1768</v>
+      </c>
+      <c r="B429" t="s">
+        <v>598</v>
+      </c>
+      <c r="C429" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>37</v>
+      </c>
+      <c r="B430" t="s">
+        <v>601</v>
+      </c>
+      <c r="C430" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>142</v>
+      </c>
+      <c r="B431" t="s">
+        <v>601</v>
+      </c>
+      <c r="C431" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>645</v>
+      </c>
+      <c r="B432" t="s">
+        <v>604</v>
+      </c>
+      <c r="C432" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>3541</v>
+      </c>
+      <c r="B433" t="s">
+        <v>604</v>
+      </c>
+      <c r="C433" s="23" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>93</v>
+      </c>
+      <c r="B434" t="s">
+        <v>604</v>
+      </c>
+      <c r="C434" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>118</v>
+      </c>
+      <c r="B435" t="s">
+        <v>604</v>
+      </c>
+      <c r="C435" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A436" s="3">
+        <v>1904</v>
+      </c>
+      <c r="B436" t="s">
+        <v>608</v>
+      </c>
+      <c r="C436" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A437" s="3">
+        <v>1905</v>
+      </c>
+      <c r="B437" t="s">
+        <v>608</v>
+      </c>
+      <c r="C437" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>1906</v>
+      </c>
+      <c r="B438" t="s">
+        <v>608</v>
+      </c>
+      <c r="C438" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>1907</v>
+      </c>
+      <c r="B439" t="s">
+        <v>608</v>
+      </c>
+      <c r="C439" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>1908</v>
+      </c>
+      <c r="B440" t="s">
+        <v>608</v>
+      </c>
+      <c r="C440" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>1909</v>
+      </c>
+      <c r="B441" t="s">
+        <v>608</v>
+      </c>
+      <c r="C441" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <v>1910</v>
+      </c>
+      <c r="B442" t="s">
+        <v>608</v>
+      </c>
+      <c r="C442" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <v>1911</v>
+      </c>
+      <c r="B443" t="s">
+        <v>608</v>
+      </c>
+      <c r="C443" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <v>3587</v>
+      </c>
+      <c r="B444" t="s">
+        <v>608</v>
+      </c>
+      <c r="C444" s="23" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <v>3588</v>
+      </c>
+      <c r="B445" t="s">
+        <v>608</v>
+      </c>
+      <c r="C445" s="23" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <v>3589</v>
+      </c>
+      <c r="B446" t="s">
+        <v>608</v>
+      </c>
+      <c r="C446" s="23" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <v>3590</v>
+      </c>
+      <c r="B447" t="s">
+        <v>608</v>
+      </c>
+      <c r="C447" s="23" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <v>3591</v>
+      </c>
+      <c r="B448" t="s">
+        <v>608</v>
+      </c>
+      <c r="C448" s="23" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A449" s="3">
+        <v>3592</v>
+      </c>
+      <c r="B449" t="s">
+        <v>608</v>
+      </c>
+      <c r="C449" s="23" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A450">
+        <v>3631</v>
+      </c>
+      <c r="B450" s="23" t="s">
+        <v>610</v>
+      </c>
+      <c r="C450" s="23" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A451">
+        <v>3651</v>
+      </c>
+      <c r="B451" t="s">
+        <v>614</v>
+      </c>
+      <c r="C451" s="23" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A452">
+        <v>3652</v>
+      </c>
+      <c r="B452" t="s">
+        <v>614</v>
+      </c>
+      <c r="C452" s="23" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A453">
+        <v>3653</v>
+      </c>
+      <c r="B453" t="s">
+        <v>614</v>
+      </c>
+      <c r="C453" s="23" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A454">
+        <v>3654</v>
+      </c>
+      <c r="B454" t="s">
+        <v>614</v>
+      </c>
+      <c r="C454" s="23" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A455">
+        <v>3661</v>
+      </c>
+      <c r="B455" t="s">
+        <v>614</v>
+      </c>
+      <c r="C455" s="23" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A456" s="3">
+        <v>3662</v>
+      </c>
+      <c r="B456" t="s">
+        <v>614</v>
+      </c>
+      <c r="C456" s="23" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A457">
+        <v>3663</v>
+      </c>
+      <c r="B457" t="s">
+        <v>614</v>
+      </c>
+      <c r="C457" s="23" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A458">
+        <v>3664</v>
+      </c>
+      <c r="B458" t="s">
+        <v>614</v>
+      </c>
+      <c r="C458" s="23" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A459">
+        <v>124</v>
+      </c>
+      <c r="B459" t="s">
+        <v>614</v>
+      </c>
+      <c r="C459" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A460">
+        <v>1669</v>
+      </c>
+      <c r="B460" t="s">
+        <v>614</v>
+      </c>
+      <c r="C460" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A461">
+        <v>1670</v>
+      </c>
+      <c r="B461" t="s">
+        <v>614</v>
+      </c>
+      <c r="C461" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <v>1671</v>
+      </c>
+      <c r="B462" t="s">
+        <v>614</v>
+      </c>
+      <c r="C462" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <v>1672</v>
+      </c>
+      <c r="B463" t="s">
+        <v>614</v>
+      </c>
+      <c r="C463" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <v>1673</v>
+      </c>
+      <c r="B464" t="s">
+        <v>614</v>
+      </c>
+      <c r="C464" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A465" s="3">
+        <v>1674</v>
+      </c>
+      <c r="B465" t="s">
+        <v>614</v>
+      </c>
+      <c r="C465" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A466" s="3">
+        <v>1675</v>
+      </c>
+      <c r="B466" t="s">
+        <v>614</v>
+      </c>
+      <c r="C466" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <v>1676</v>
+      </c>
+      <c r="B467" t="s">
+        <v>614</v>
+      </c>
+      <c r="C467" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <v>1677</v>
+      </c>
+      <c r="B468" t="s">
+        <v>614</v>
+      </c>
+      <c r="C468" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A469">
+        <v>1678</v>
+      </c>
+      <c r="B469" t="s">
+        <v>614</v>
+      </c>
+      <c r="C469" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A470">
+        <v>1679</v>
+      </c>
+      <c r="B470" t="s">
+        <v>614</v>
+      </c>
+      <c r="C470" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A471">
+        <v>3717</v>
+      </c>
+      <c r="B471" t="s">
+        <v>618</v>
+      </c>
+      <c r="C471" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A472">
+        <v>3722</v>
+      </c>
+      <c r="B472" t="s">
+        <v>618</v>
+      </c>
+      <c r="C472" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A473">
+        <v>3723</v>
+      </c>
+      <c r="B473" t="s">
+        <v>618</v>
+      </c>
+      <c r="C473" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A474">
+        <v>3724</v>
+      </c>
+      <c r="B474" t="s">
+        <v>618</v>
+      </c>
+      <c r="C474" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A475" s="3">
+        <v>3725</v>
+      </c>
+      <c r="B475" t="s">
+        <v>618</v>
+      </c>
+      <c r="C475" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A476">
+        <v>3726</v>
+      </c>
+      <c r="B476" t="s">
+        <v>618</v>
+      </c>
+      <c r="C476" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A477">
+        <v>3727</v>
+      </c>
+      <c r="B477" t="s">
+        <v>618</v>
+      </c>
+      <c r="C477" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A478">
+        <v>3728</v>
+      </c>
+      <c r="B478" t="s">
+        <v>618</v>
+      </c>
+      <c r="C478" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A479">
+        <v>3729</v>
+      </c>
+      <c r="B479" t="s">
+        <v>618</v>
+      </c>
+      <c r="C479" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A480">
+        <v>3730</v>
+      </c>
+      <c r="B480" t="s">
+        <v>618</v>
+      </c>
+      <c r="C480" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A481">
+        <v>3731</v>
+      </c>
+      <c r="B481" t="s">
+        <v>618</v>
+      </c>
+      <c r="C481" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A482" s="3">
+        <v>3732</v>
+      </c>
+      <c r="B482" t="s">
+        <v>618</v>
+      </c>
+      <c r="C482" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A483">
+        <v>3733</v>
+      </c>
+      <c r="B483" t="s">
+        <v>618</v>
+      </c>
+      <c r="C483" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A484">
+        <v>3734</v>
+      </c>
+      <c r="B484" t="s">
+        <v>618</v>
+      </c>
+      <c r="C484" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A485">
+        <v>3735</v>
+      </c>
+      <c r="B485" t="s">
+        <v>618</v>
+      </c>
+      <c r="C485" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A486">
+        <v>3736</v>
+      </c>
+      <c r="B486" t="s">
+        <v>618</v>
+      </c>
+      <c r="C486" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A487">
+        <v>3737</v>
+      </c>
+      <c r="B487" t="s">
+        <v>618</v>
+      </c>
+      <c r="C487" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A488">
+        <v>3738</v>
+      </c>
+      <c r="B488" t="s">
+        <v>618</v>
+      </c>
+      <c r="C488" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A489" s="3">
+        <v>3739</v>
+      </c>
+      <c r="B489" t="s">
+        <v>618</v>
+      </c>
+      <c r="C489" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A490">
+        <v>3740</v>
+      </c>
+      <c r="B490" t="s">
+        <v>618</v>
+      </c>
+      <c r="C490" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A491">
+        <v>3741</v>
+      </c>
+      <c r="B491" t="s">
+        <v>618</v>
+      </c>
+      <c r="C491" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A492">
+        <v>3742</v>
+      </c>
+      <c r="B492" t="s">
+        <v>618</v>
+      </c>
+      <c r="C492" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A493">
+        <v>3743</v>
+      </c>
+      <c r="B493" t="s">
+        <v>618</v>
+      </c>
+      <c r="C493" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A494">
+        <v>3744</v>
+      </c>
+      <c r="B494" t="s">
+        <v>618</v>
+      </c>
+      <c r="C494" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A495">
+        <v>3745</v>
+      </c>
+      <c r="B495" t="s">
+        <v>618</v>
+      </c>
+      <c r="C495" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A496" s="3">
+        <v>3746</v>
+      </c>
+      <c r="B496" t="s">
+        <v>618</v>
+      </c>
+      <c r="C496" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A497">
+        <v>3747</v>
+      </c>
+      <c r="B497" t="s">
+        <v>618</v>
+      </c>
+      <c r="C497" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A498">
+        <v>3748</v>
+      </c>
+      <c r="B498" t="s">
+        <v>618</v>
+      </c>
+      <c r="C498" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A499">
+        <v>3749</v>
+      </c>
+      <c r="B499" t="s">
+        <v>618</v>
+      </c>
+      <c r="C499" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A500">
+        <v>3750</v>
+      </c>
+      <c r="B500" t="s">
+        <v>618</v>
+      </c>
+      <c r="C500" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A501">
+        <v>3751</v>
+      </c>
+      <c r="B501" t="s">
+        <v>618</v>
+      </c>
+      <c r="C501" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A502">
+        <v>3752</v>
+      </c>
+      <c r="B502" t="s">
+        <v>618</v>
+      </c>
+      <c r="C502" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A503" s="3">
+        <v>3753</v>
+      </c>
+      <c r="B503" t="s">
+        <v>618</v>
+      </c>
+      <c r="C503" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A504">
+        <v>3754</v>
+      </c>
+      <c r="B504" t="s">
+        <v>618</v>
+      </c>
+      <c r="C504" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A505">
+        <v>3755</v>
+      </c>
+      <c r="B505" t="s">
+        <v>618</v>
+      </c>
+      <c r="C505" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A506">
+        <v>3756</v>
+      </c>
+      <c r="B506" t="s">
+        <v>618</v>
+      </c>
+      <c r="C506" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A507">
+        <v>3757</v>
+      </c>
+      <c r="B507" t="s">
+        <v>618</v>
+      </c>
+      <c r="C507" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A508">
+        <v>3758</v>
+      </c>
+      <c r="B508" t="s">
+        <v>618</v>
+      </c>
+      <c r="C508" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A509">
+        <v>3759</v>
+      </c>
+      <c r="B509" t="s">
+        <v>618</v>
+      </c>
+      <c r="C509" s="23" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A510">
+        <v>616</v>
+      </c>
+      <c r="B510" t="s">
+        <v>620</v>
+      </c>
+      <c r="C510" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A511">
+        <v>1230</v>
+      </c>
+      <c r="B511" t="s">
+        <v>624</v>
+      </c>
+      <c r="C511" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A512">
+        <v>1231</v>
+      </c>
+      <c r="B512" t="s">
+        <v>624</v>
+      </c>
+      <c r="C512" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A513" s="3">
+        <v>1232</v>
+      </c>
+      <c r="B513" t="s">
+        <v>624</v>
+      </c>
+      <c r="C513" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A514">
+        <v>1350</v>
+      </c>
+      <c r="B514" t="s">
+        <v>628</v>
+      </c>
+      <c r="C514" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A515">
+        <v>3783</v>
+      </c>
+      <c r="B515" t="s">
+        <v>628</v>
+      </c>
+      <c r="C515" s="23" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A516">
+        <v>3784</v>
+      </c>
+      <c r="B516" t="s">
+        <v>628</v>
+      </c>
+      <c r="C516" s="23" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A517">
+        <v>3785</v>
+      </c>
+      <c r="B517" t="s">
+        <v>628</v>
+      </c>
+      <c r="C517" s="23" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A518">
+        <v>47</v>
+      </c>
+      <c r="B518" t="s">
+        <v>630</v>
+      </c>
+      <c r="C518" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A519">
+        <v>671</v>
+      </c>
+      <c r="B519" t="s">
+        <v>630</v>
+      </c>
+      <c r="C519" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A520">
+        <v>841</v>
+      </c>
+      <c r="B520" t="s">
+        <v>630</v>
+      </c>
+      <c r="C520" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A521">
+        <v>843</v>
+      </c>
+      <c r="B521" t="s">
+        <v>630</v>
+      </c>
+      <c r="C521" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A522">
+        <v>863</v>
+      </c>
+      <c r="B522" t="s">
+        <v>630</v>
+      </c>
+      <c r="C522" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A523">
+        <v>3780</v>
+      </c>
+      <c r="B523" t="s">
+        <v>630</v>
+      </c>
+      <c r="C523" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A524">
+        <v>72</v>
+      </c>
+      <c r="B524" t="s">
+        <v>632</v>
+      </c>
+      <c r="C524" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A525">
+        <v>447</v>
+      </c>
+      <c r="B525" t="s">
+        <v>632</v>
+      </c>
+      <c r="C525" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A526">
+        <v>1425</v>
+      </c>
+      <c r="B526" t="s">
+        <v>632</v>
+      </c>
+      <c r="C526" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A527">
+        <v>1426</v>
+      </c>
+      <c r="B527" t="s">
+        <v>632</v>
+      </c>
+      <c r="C527" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A528">
+        <v>1427</v>
+      </c>
+      <c r="B528" t="s">
+        <v>632</v>
+      </c>
+      <c r="C528" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A529" s="3">
+        <v>1428</v>
+      </c>
+      <c r="B529" t="s">
+        <v>632</v>
+      </c>
+      <c r="C529" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A530">
+        <v>3796</v>
+      </c>
+      <c r="B530" t="s">
+        <v>632</v>
+      </c>
+      <c r="C530" s="23" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A531">
+        <v>3802</v>
+      </c>
+      <c r="B531" t="s">
+        <v>632</v>
+      </c>
+      <c r="C531" s="23" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A532">
+        <v>1407</v>
+      </c>
+      <c r="B532" t="s">
+        <v>636</v>
+      </c>
+      <c r="C532" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A533">
+        <v>1220</v>
+      </c>
+      <c r="B533" t="s">
+        <v>638</v>
+      </c>
+      <c r="C533" t="s">
+        <v>637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Steur updated to 1760
</commit_message>
<xml_diff>
--- a/Data/Extra info verwijderde namen.xlsx
+++ b/Data/Extra info verwijderde namen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alielassche/Documents/GitHub/netwerk-huwelijksgedichten/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBE6911-F87E-A34E-B1EB-785142F107E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA670A0B-5421-204B-9C95-EDBE7344D38A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{91DC8FCD-999E-C04C-A5B7-D30830052C4B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="640">
   <si>
     <t>Goeree</t>
   </si>
@@ -1945,6 +1945,9 @@
   </si>
   <si>
     <t>Reinier Leers</t>
+  </si>
+  <si>
+    <t>L. Groenewolt (wed.)</t>
   </si>
 </sst>
 </file>
@@ -2426,10 +2429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC8214C-B4FA-7B44-AB5D-D8A034BCE402}">
-  <dimension ref="A1:D533"/>
+  <dimension ref="A1:D535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A383" workbookViewId="0">
-      <selection activeCell="B401" sqref="B401"/>
+    <sheetView tabSelected="1" topLeftCell="A524" workbookViewId="0">
+      <selection activeCell="C539" sqref="C539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8374,6 +8377,17 @@
       </c>
       <c r="C533" t="s">
         <v>637</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A535">
+        <v>4024</v>
+      </c>
+      <c r="B535" t="s">
+        <v>66</v>
+      </c>
+      <c r="C535" t="s">
+        <v>639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>